<commit_message>
end of day 1 validation push
one third done
</commit_message>
<xml_diff>
--- a/Lit review data/lit review master COMBINED.xlsx
+++ b/Lit review data/lit review master COMBINED.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8075" uniqueCount="2589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15714" uniqueCount="2591">
   <si>
     <t>Latin name</t>
   </si>
@@ -30854,15 +30854,28 @@
   </si>
   <si>
     <t>prevalence modelling, risk mapping, cluster analysis</t>
+  </si>
+  <si>
+    <t>cjc flag - also "helminthiasis"</t>
+  </si>
+  <si>
+    <t>cjc flag - nice summary of WHO guidelines for intervention</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31091,92 +31104,95 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -31496,9 +31512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X525"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E139" sqref="E139"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -38492,6 +38508,12 @@
       <c r="C128" s="25">
         <v>2009</v>
       </c>
+      <c r="D128" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E128" s="39" t="s">
+        <v>2570</v>
+      </c>
       <c r="F128" t="s">
         <v>1083</v>
       </c>
@@ -38536,6 +38558,12 @@
       <c r="C129" s="25">
         <v>2018</v>
       </c>
+      <c r="D129" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E129" s="39" t="s">
+        <v>2586</v>
+      </c>
       <c r="F129" s="25" t="s">
         <v>699</v>
       </c>
@@ -38586,6 +38614,12 @@
       <c r="C130" s="25">
         <v>2006</v>
       </c>
+      <c r="D130" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E130" s="39" t="s">
+        <v>2571</v>
+      </c>
       <c r="F130" t="s">
         <v>701</v>
       </c>
@@ -38645,6 +38679,12 @@
       <c r="C131" s="25">
         <v>2007</v>
       </c>
+      <c r="D131" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E131" s="39" t="s">
+        <v>2571</v>
+      </c>
       <c r="F131" t="s">
         <v>700</v>
       </c>
@@ -38695,6 +38735,12 @@
       <c r="C132" s="25">
         <v>2008</v>
       </c>
+      <c r="D132" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E132" s="39" t="s">
+        <v>2570</v>
+      </c>
       <c r="F132" s="25" t="s">
         <v>704</v>
       </c>
@@ -38748,6 +38794,12 @@
       <c r="C133" s="25">
         <v>2015</v>
       </c>
+      <c r="D133" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E133" s="39" t="s">
+        <v>2566</v>
+      </c>
       <c r="F133" s="25" t="s">
         <v>681</v>
       </c>
@@ -38804,6 +38856,12 @@
       <c r="C134" s="25">
         <v>2013</v>
       </c>
+      <c r="D134" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E134" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F134" s="25" t="s">
         <v>724</v>
       </c>
@@ -38860,6 +38918,12 @@
       <c r="C135" s="25">
         <v>2018</v>
       </c>
+      <c r="D135" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E135" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F135" s="25" t="s">
         <v>735</v>
       </c>
@@ -38913,6 +38977,12 @@
       <c r="C136" s="25">
         <v>2014</v>
       </c>
+      <c r="D136" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E136" s="39" t="s">
+        <v>2581</v>
+      </c>
       <c r="F136" t="s">
         <v>740</v>
       </c>
@@ -38963,6 +39033,12 @@
       <c r="C137" s="25">
         <v>2018</v>
       </c>
+      <c r="D137" s="38" t="s">
+        <v>2589</v>
+      </c>
+      <c r="E137" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F137" t="s">
         <v>745</v>
       </c>
@@ -39010,6 +39086,12 @@
       <c r="C138" s="25">
         <v>2011</v>
       </c>
+      <c r="D138" s="38" t="s">
+        <v>2590</v>
+      </c>
+      <c r="E138" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F138" t="s">
         <v>781</v>
       </c>
@@ -39063,6 +39145,12 @@
       <c r="C139" s="25">
         <v>2014</v>
       </c>
+      <c r="D139" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E139" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F139" s="25" t="s">
         <v>787</v>
       </c>
@@ -39116,7 +39204,13 @@
       <c r="C140" s="25">
         <v>2014</v>
       </c>
-      <c r="F140" t="s">
+      <c r="D140" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E140" s="39" t="s">
+        <v>2151</v>
+      </c>
+      <c r="F140" s="4" t="s">
         <v>797</v>
       </c>
       <c r="G140" s="25" t="s">
@@ -39169,6 +39263,12 @@
       <c r="C141" s="25">
         <v>2017</v>
       </c>
+      <c r="D141" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E141" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F141" s="25" t="s">
         <v>789</v>
       </c>
@@ -39222,6 +39322,12 @@
       <c r="C142" s="25">
         <v>2014</v>
       </c>
+      <c r="D142" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E142" s="39" t="s">
+        <v>2581</v>
+      </c>
       <c r="F142" s="25" t="s">
         <v>806</v>
       </c>
@@ -39272,6 +39378,12 @@
       <c r="C143" s="25">
         <v>2012</v>
       </c>
+      <c r="D143" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E143" s="39" t="s">
+        <v>2566</v>
+      </c>
       <c r="F143" s="25" t="s">
         <v>829</v>
       </c>
@@ -39328,6 +39440,12 @@
       <c r="C144" s="25">
         <v>2010</v>
       </c>
+      <c r="D144" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E144" s="39" t="s">
+        <v>2582</v>
+      </c>
       <c r="F144" s="25" t="s">
         <v>826</v>
       </c>
@@ -39381,6 +39499,12 @@
       <c r="C145" s="25">
         <v>2012</v>
       </c>
+      <c r="D145" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E145" s="39" t="s">
+        <v>2572</v>
+      </c>
       <c r="F145" s="25" t="s">
         <v>831</v>
       </c>
@@ -39431,6 +39555,12 @@
       <c r="C146" s="25">
         <v>2015</v>
       </c>
+      <c r="D146" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E146" s="39" t="s">
+        <v>2574</v>
+      </c>
       <c r="F146" s="25" t="s">
         <v>834</v>
       </c>
@@ -39481,6 +39611,12 @@
       <c r="C147" s="25">
         <v>2017</v>
       </c>
+      <c r="D147" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E147" s="39" t="s">
+        <v>2566</v>
+      </c>
       <c r="F147" s="25" t="s">
         <v>843</v>
       </c>
@@ -39531,6 +39667,12 @@
       <c r="C148" s="25">
         <v>2017</v>
       </c>
+      <c r="D148" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E148" s="39" t="s">
+        <v>2572</v>
+      </c>
       <c r="F148" s="25" t="s">
         <v>846</v>
       </c>
@@ -39584,6 +39726,12 @@
       <c r="C149" s="25">
         <v>2018</v>
       </c>
+      <c r="D149" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E149" s="39" t="s">
+        <v>2569</v>
+      </c>
       <c r="F149" s="25" t="s">
         <v>851</v>
       </c>
@@ -39634,6 +39782,12 @@
       <c r="C150" s="25">
         <v>2012</v>
       </c>
+      <c r="D150" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E150" s="39" t="s">
+        <v>2568</v>
+      </c>
       <c r="F150" s="25" t="s">
         <v>856</v>
       </c>
@@ -39681,6 +39835,12 @@
       <c r="C151" s="25">
         <v>2016</v>
       </c>
+      <c r="D151" s="39" t="s">
+        <v>2584</v>
+      </c>
+      <c r="E151" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F151" t="s">
         <v>859</v>
       </c>
@@ -39737,6 +39897,12 @@
       <c r="C152" s="25">
         <v>2017</v>
       </c>
+      <c r="D152" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E152" s="39" t="s">
+        <v>2570</v>
+      </c>
       <c r="F152" s="25" t="s">
         <v>861</v>
       </c>
@@ -39787,6 +39953,12 @@
       <c r="C153" s="25">
         <v>2013</v>
       </c>
+      <c r="D153" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E153" s="39" t="s">
+        <v>2585</v>
+      </c>
       <c r="F153" s="25" t="s">
         <v>862</v>
       </c>
@@ -39837,6 +40009,12 @@
       <c r="C154" s="25">
         <v>2004</v>
       </c>
+      <c r="D154" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E154" s="39" t="s">
+        <v>2570</v>
+      </c>
       <c r="F154" t="s">
         <v>1110</v>
       </c>
@@ -39887,6 +40065,12 @@
       <c r="C155" s="25">
         <v>2015</v>
       </c>
+      <c r="D155" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E155" s="39" t="s">
+        <v>2568</v>
+      </c>
       <c r="F155" t="s">
         <v>915</v>
       </c>
@@ -39937,6 +40121,12 @@
       <c r="C156" s="25">
         <v>2012</v>
       </c>
+      <c r="D156" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E156" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F156" t="s">
         <v>923</v>
       </c>
@@ -39990,6 +40180,12 @@
       <c r="C157" s="25">
         <v>2012</v>
       </c>
+      <c r="D157" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E157" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F157" t="s">
         <v>925</v>
       </c>
@@ -40043,6 +40239,12 @@
       <c r="C158" s="25">
         <v>2012</v>
       </c>
+      <c r="D158" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E158" s="39" t="s">
+        <v>2573</v>
+      </c>
       <c r="F158" t="s">
         <v>926</v>
       </c>
@@ -40096,6 +40298,12 @@
       <c r="C159" s="25">
         <v>2017</v>
       </c>
+      <c r="D159" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E159" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F159" t="s">
         <v>909</v>
       </c>
@@ -40143,6 +40351,12 @@
       <c r="C160" s="25">
         <v>2018</v>
       </c>
+      <c r="D160" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E160" s="39" t="s">
+        <v>2568</v>
+      </c>
       <c r="F160" s="25" t="s">
         <v>892</v>
       </c>
@@ -40196,6 +40410,12 @@
       <c r="C161" s="25">
         <v>2018</v>
       </c>
+      <c r="D161" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E161" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F161" s="30" t="s">
         <v>945</v>
       </c>
@@ -40249,6 +40469,12 @@
       <c r="C162" s="25">
         <v>2004</v>
       </c>
+      <c r="D162" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E162" s="39" t="s">
+        <v>2573</v>
+      </c>
       <c r="F162" t="s">
         <v>939</v>
       </c>
@@ -40299,6 +40525,12 @@
       <c r="C163" s="25">
         <v>2006</v>
       </c>
+      <c r="D163" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E163" s="39" t="s">
+        <v>2159</v>
+      </c>
       <c r="F163" t="s">
         <v>930</v>
       </c>
@@ -40349,6 +40581,9 @@
       <c r="C164" s="25">
         <v>2010</v>
       </c>
+      <c r="D164" s="38" t="s">
+        <v>2576</v>
+      </c>
       <c r="F164" t="s">
         <v>928</v>
       </c>
@@ -40399,6 +40634,12 @@
       <c r="C165" s="25">
         <v>2011</v>
       </c>
+      <c r="D165" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E165" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F165" s="25" t="s">
         <v>868</v>
       </c>
@@ -40452,6 +40693,12 @@
       <c r="C166" s="25">
         <v>2011</v>
       </c>
+      <c r="D166" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E166" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F166" t="s">
         <v>870</v>
       </c>
@@ -40502,6 +40749,12 @@
       <c r="C167" s="25">
         <v>2011</v>
       </c>
+      <c r="D167" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E167" s="39" t="s">
+        <v>2566</v>
+      </c>
       <c r="F167" t="s">
         <v>1118</v>
       </c>
@@ -40552,6 +40805,12 @@
       <c r="C168" s="25">
         <v>2014</v>
       </c>
+      <c r="D168" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E168" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F168" s="25" t="s">
         <v>876</v>
       </c>
@@ -40602,6 +40861,9 @@
       <c r="C169" s="25">
         <v>2016</v>
       </c>
+      <c r="D169" s="38" t="s">
+        <v>2576</v>
+      </c>
       <c r="F169" t="s">
         <v>898</v>
       </c>
@@ -40655,6 +40917,12 @@
       <c r="C170" s="25">
         <v>2017</v>
       </c>
+      <c r="D170" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E170" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F170" s="25" t="s">
         <v>884</v>
       </c>
@@ -40708,6 +40976,12 @@
       <c r="C171" s="25">
         <v>2017</v>
       </c>
+      <c r="D171" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E171" s="39" t="s">
+        <v>2568</v>
+      </c>
       <c r="F171" t="s">
         <v>897</v>
       </c>
@@ -40761,6 +41035,12 @@
       <c r="C172" s="25">
         <v>2017</v>
       </c>
+      <c r="D172" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E172" s="39" t="s">
+        <v>2568</v>
+      </c>
       <c r="F172" t="s">
         <v>911</v>
       </c>
@@ -40808,6 +41088,12 @@
       <c r="C173" s="25">
         <v>2018</v>
       </c>
+      <c r="D173" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E173" s="39" t="s">
+        <v>2568</v>
+      </c>
       <c r="F173" t="s">
         <v>896</v>
       </c>
@@ -40861,6 +41147,12 @@
       <c r="C174" s="25">
         <v>2018</v>
       </c>
+      <c r="D174" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E174" s="39" t="s">
+        <v>2151</v>
+      </c>
       <c r="F174" t="s">
         <v>903</v>
       </c>
@@ -40907,6 +41199,12 @@
       </c>
       <c r="C175" s="25">
         <v>2019</v>
+      </c>
+      <c r="D175" s="39" t="s">
+        <v>2565</v>
+      </c>
+      <c r="E175" s="39" t="s">
+        <v>2570</v>
       </c>
       <c r="F175" t="s">
         <v>902</v>
@@ -57234,9 +57532,10 @@
     <hyperlink ref="W472" r:id="rId3" display="https://data.mendeley.com/datasets/vch6n3pd8f/1"/>
     <hyperlink ref="F83" r:id="rId4"/>
     <hyperlink ref="F96" r:id="rId5"/>
+    <hyperlink ref="F140" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -58494,8 +58793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
100 left for sunday
</commit_message>
<xml_diff>
--- a/Lit review data/lit review master COMBINED.xlsx
+++ b/Lit review data/lit review master COMBINED.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15659" uniqueCount="2611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8651" uniqueCount="2611">
   <si>
     <t>Latin name</t>
   </si>
@@ -28638,9 +28638,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28906,107 +28913,110 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -29326,9 +29336,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X525"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A399" zoomScale="93" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A404" zoomScale="93" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D401" sqref="D401"/>
+      <selection pane="topRight" activeCell="E424" sqref="E424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -50966,6 +50976,12 @@
       <c r="C401" s="24">
         <v>2016</v>
       </c>
+      <c r="D401" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E401" s="44" t="s">
+        <v>2074</v>
+      </c>
       <c r="F401" t="s">
         <v>1094</v>
       </c>
@@ -51013,6 +51029,12 @@
       <c r="C402" s="24">
         <v>2008</v>
       </c>
+      <c r="D402" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E402" s="44" t="s">
+        <v>2490</v>
+      </c>
       <c r="F402" t="s">
         <v>1103</v>
       </c>
@@ -51045,6 +51067,12 @@
       <c r="C403" s="24">
         <v>2012</v>
       </c>
+      <c r="D403" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E403" s="44" t="s">
+        <v>2490</v>
+      </c>
       <c r="F403" t="s">
         <v>1100</v>
       </c>
@@ -51080,6 +51108,12 @@
       <c r="C404" s="24">
         <v>2014</v>
       </c>
+      <c r="D404" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E404" s="44" t="s">
+        <v>2492</v>
+      </c>
       <c r="F404" t="s">
         <v>933</v>
       </c>
@@ -51136,6 +51170,12 @@
       <c r="C405" s="24">
         <v>2011</v>
       </c>
+      <c r="D405" s="41" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E405" s="41" t="s">
+        <v>2493</v>
+      </c>
       <c r="F405" t="s">
         <v>897</v>
       </c>
@@ -51195,6 +51235,12 @@
       <c r="C406" s="24">
         <v>2003</v>
       </c>
+      <c r="D406" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E406" s="44" t="s">
+        <v>2074</v>
+      </c>
       <c r="F406" t="s">
         <v>928</v>
       </c>
@@ -51248,6 +51294,12 @@
       <c r="C407" s="24">
         <v>2011</v>
       </c>
+      <c r="D407" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E407" s="44" t="s">
+        <v>2089</v>
+      </c>
       <c r="F407" s="24" t="s">
         <v>863</v>
       </c>
@@ -51301,7 +51353,13 @@
       <c r="C408" s="24">
         <v>2011</v>
       </c>
-      <c r="F408" t="s">
+      <c r="D408" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E408" s="44" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F408" s="4" t="s">
         <v>868</v>
       </c>
       <c r="G408" s="24" t="s">
@@ -51351,6 +51409,12 @@
       <c r="C409" s="24">
         <v>2013</v>
       </c>
+      <c r="D409" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E409" s="44" t="s">
+        <v>2075</v>
+      </c>
       <c r="F409" t="s">
         <v>917</v>
       </c>
@@ -51398,6 +51462,12 @@
       <c r="C410" s="24">
         <v>2013</v>
       </c>
+      <c r="D410" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E410" s="44" t="s">
+        <v>2075</v>
+      </c>
       <c r="F410" t="s">
         <v>918</v>
       </c>
@@ -51448,6 +51518,12 @@
       <c r="C411" s="24">
         <v>2015</v>
       </c>
+      <c r="D411" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E411" s="44" t="s">
+        <v>2074</v>
+      </c>
       <c r="F411" s="24" t="s">
         <v>875</v>
       </c>
@@ -51498,6 +51574,12 @@
       <c r="C412" s="24">
         <v>2015</v>
       </c>
+      <c r="D412" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E412" s="44" t="s">
+        <v>2075</v>
+      </c>
       <c r="F412" t="s">
         <v>911</v>
       </c>
@@ -51548,6 +51630,12 @@
       <c r="C413" s="24">
         <v>2017</v>
       </c>
+      <c r="D413" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E413" s="44" t="s">
+        <v>2089</v>
+      </c>
       <c r="F413" s="24" t="s">
         <v>883</v>
       </c>
@@ -51595,6 +51683,12 @@
       <c r="C414" s="24">
         <v>2017</v>
       </c>
+      <c r="D414" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E414" s="44" t="s">
+        <v>2074</v>
+      </c>
       <c r="F414" t="s">
         <v>902</v>
       </c>
@@ -51648,6 +51742,12 @@
       <c r="C415" s="24">
         <v>2017</v>
       </c>
+      <c r="D415" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E415" s="44" t="s">
+        <v>2075</v>
+      </c>
       <c r="F415" t="s">
         <v>909</v>
       </c>
@@ -51698,6 +51798,12 @@
       <c r="C416" s="24">
         <v>2018</v>
       </c>
+      <c r="D416" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E416" s="44" t="s">
+        <v>2089</v>
+      </c>
       <c r="F416" s="24" t="s">
         <v>891</v>
       </c>
@@ -51748,6 +51854,12 @@
       <c r="C417" s="24">
         <v>2018</v>
       </c>
+      <c r="D417" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E417" s="44" t="s">
+        <v>2596</v>
+      </c>
       <c r="F417" t="s">
         <v>892</v>
       </c>
@@ -51798,6 +51910,12 @@
       <c r="C418" s="24">
         <v>2018</v>
       </c>
+      <c r="D418" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E418" s="44" t="s">
+        <v>2075</v>
+      </c>
       <c r="F418" t="s">
         <v>901</v>
       </c>
@@ -51848,6 +51966,12 @@
       <c r="C419" s="24">
         <v>2007</v>
       </c>
+      <c r="D419" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E419" s="44" t="s">
+        <v>2492</v>
+      </c>
       <c r="F419" t="s">
         <v>926</v>
       </c>
@@ -51898,6 +52022,12 @@
       <c r="C420" s="24">
         <v>2012</v>
       </c>
+      <c r="D420" s="41" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E420" s="41" t="s">
+        <v>2493</v>
+      </c>
       <c r="F420" t="s">
         <v>870</v>
       </c>
@@ -51951,6 +52081,12 @@
       <c r="C421" s="24">
         <v>2012</v>
       </c>
+      <c r="D421" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E421" s="44" t="s">
+        <v>2490</v>
+      </c>
       <c r="F421" t="s">
         <v>921</v>
       </c>
@@ -51995,6 +52131,12 @@
       <c r="C422" s="24">
         <v>2013</v>
       </c>
+      <c r="D422" s="41" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E422" s="41" t="s">
+        <v>2493</v>
+      </c>
       <c r="F422" s="24" t="s">
         <v>945</v>
       </c>
@@ -52045,6 +52187,12 @@
       <c r="C423" s="24">
         <v>2014</v>
       </c>
+      <c r="D423" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E423" s="44" t="s">
+        <v>2074</v>
+      </c>
       <c r="F423" t="s">
         <v>332</v>
       </c>
@@ -52086,6 +52234,9 @@
       <c r="C424" s="24">
         <v>2014</v>
       </c>
+      <c r="D424" s="36" t="s">
+        <v>2522</v>
+      </c>
       <c r="F424" t="s">
         <v>334</v>
       </c>
@@ -52132,6 +52283,12 @@
       </c>
       <c r="C425" s="24">
         <v>2014</v>
+      </c>
+      <c r="D425" s="44" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E425" s="44" t="s">
+        <v>2129</v>
       </c>
       <c r="F425" s="24" t="s">
         <v>872</v>
@@ -56660,9 +56817,10 @@
     <hyperlink ref="F379" r:id="rId18"/>
     <hyperlink ref="F384" r:id="rId19"/>
     <hyperlink ref="F397" r:id="rId20"/>
+    <hyperlink ref="F408" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>